<commit_message>
adjust 9mm barrels & muzzles + radian parts
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED78244-5E31-4470-95CA-9C5F14201B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C714C9-859C-41CE-9A7E-41201A41014D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="4590" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>new</t>
   </si>
@@ -62,9 +62,6 @@
     <t>magazine_capacity</t>
   </si>
   <si>
-    <t>bullet_deviation</t>
-  </si>
-  <si>
     <t>bullet_damage</t>
   </si>
   <si>
@@ -204,6 +201,15 @@
   </si>
   <si>
     <t xml:space="preserve">HK USC 9x19 16.5" </t>
+  </si>
+  <si>
+    <t>radian_weapons_glock17_ramjet_barrel</t>
+  </si>
+  <si>
+    <t>Radian Weapons Glock 17 Gen5 RAMJET 9x19</t>
+  </si>
+  <si>
+    <t>barrel_deviation</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,45 +1103,45 @@
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>16</v>
-      </c>
-      <c r="U2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1162,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
+        <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*15+J3/300</f>
         <v>12.996666666666666</v>
       </c>
       <c r="P3">
@@ -1178,25 +1184,25 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="E4">
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="F4">
         <v>-10</v>
       </c>
       <c r="H4">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1205,524 +1211,511 @@
         <v>-57</v>
       </c>
       <c r="M4">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N26" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
-        <v>7.96</v>
-      </c>
-      <c r="P4">
-        <v>0.06</v>
-      </c>
-      <c r="Q4">
-        <v>4.5</v>
-      </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S26" si="1">ROUND(Q4*0.023+P4+R4, 2)</f>
-        <v>0.16</v>
+        <f>C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*15+J4/300</f>
+        <v>11.31</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="E5">
-        <v>-11</v>
+        <v>-7</v>
       </c>
       <c r="F5">
-        <v>-13</v>
+        <v>-10</v>
       </c>
       <c r="H5">
-        <v>-0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I5">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>-14</v>
+        <v>-57</v>
       </c>
       <c r="M5">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="0"/>
-        <v>11.453333333333335</v>
+        <f t="shared" ref="N5:N27" si="0">C5-D5*20-E5*0.8-F5*0.6-H5*5+I5*15+J5/300</f>
+        <v>7.96</v>
       </c>
       <c r="P5">
         <v>0.06</v>
       </c>
       <c r="Q5">
+        <v>4.5</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5:S27" si="1">ROUND(Q5*0.023+P5+R5, 2)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>0.2</v>
+      </c>
+      <c r="E6">
+        <v>-12</v>
+      </c>
+      <c r="F6">
+        <v>-15</v>
+      </c>
+      <c r="H6">
+        <v>-0.1</v>
+      </c>
+      <c r="I6">
+        <v>0.05</v>
+      </c>
+      <c r="J6">
+        <v>-14</v>
+      </c>
+      <c r="M6">
+        <v>1500</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="0"/>
+        <v>14.803333333333335</v>
+      </c>
+      <c r="P6">
+        <v>0.06</v>
+      </c>
+      <c r="Q6">
         <v>6.0236200000000002</v>
       </c>
-      <c r="S5">
+      <c r="S6">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6">
+      <c r="C7">
         <v>-25</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>0.43</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>-10</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>-15</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>-0.2</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>0.1</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <v>140</v>
       </c>
-      <c r="M6">
+      <c r="M7">
         <v>3000</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N7" s="1">
         <f t="shared" si="0"/>
-        <v>-14.133333333333335</v>
-      </c>
-      <c r="P6">
+        <v>-13.633333333333335</v>
+      </c>
+      <c r="P7">
         <v>0.06</v>
       </c>
-      <c r="Q6">
+      <c r="Q7">
         <v>15.984252</v>
       </c>
-      <c r="S6">
+      <c r="S7">
         <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-3</v>
-      </c>
-      <c r="F8" s="1">
-        <v>-7</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>47</v>
-      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
+      <c r="M8" s="1"/>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
-        <v>2.0566666666666671</v>
-      </c>
-      <c r="P8">
-        <v>0.06</v>
-      </c>
-      <c r="Q8">
-        <v>8.8582699999999992</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <f t="shared" si="1"/>
-        <v>0.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>0.19</v>
+        <v>0.26</v>
       </c>
       <c r="E9" s="1">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="F9" s="1">
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I9" s="1">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="J9" s="1">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
-        <v>1.7166666666666668</v>
+        <v>2.5566666666666671</v>
       </c>
       <c r="P9">
         <v>0.06</v>
       </c>
       <c r="Q9">
-        <v>5.74803</v>
+        <v>8.8582699999999992</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-4</v>
+      </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="H10" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="J10" s="1">
+        <v>80</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="M10" s="1">
+        <v>1000</v>
+      </c>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.1166666666666667</v>
+      </c>
+      <c r="P10">
+        <v>0.06</v>
+      </c>
+      <c r="Q10">
+        <v>5.74803</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1">
-        <v>9</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="E11" s="1">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1">
-        <v>8</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I11" s="1">
-        <v>-0.3</v>
-      </c>
-      <c r="J11" s="1">
-        <v>-300</v>
-      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1">
-        <v>750</v>
-      </c>
+      <c r="M11" s="1"/>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
-        <v>-10.3</v>
-      </c>
-      <c r="P11">
-        <v>0.06</v>
-      </c>
-      <c r="Q11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>0.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="E12" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="I12" s="1">
-        <v>-0.12</v>
+        <v>-0.3</v>
       </c>
       <c r="J12" s="1">
-        <v>-225</v>
+        <v>-300</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="N12" s="1">
-        <f>C12-D12*20-E12*0.8-F12*0.6-H12*5+I12*10+J12/300</f>
-        <v>-8.1999999999999993</v>
+        <f t="shared" si="0"/>
+        <v>-11.8</v>
       </c>
       <c r="P12">
         <v>0.06</v>
       </c>
       <c r="Q12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1">
-        <v>0.26</v>
+        <v>0.18</v>
       </c>
       <c r="E13" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1">
-        <v>0.12</v>
+        <v>0.25</v>
       </c>
       <c r="I13" s="1">
-        <v>-0.04</v>
+        <v>-0.12</v>
       </c>
       <c r="J13" s="1">
-        <v>-90</v>
+        <v>-225</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="0"/>
-        <v>-7.1000000000000005</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="P13">
         <v>0.06</v>
       </c>
       <c r="Q13">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>0.26</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="E14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="J14" s="1">
-        <v>-70</v>
+        <v>-90</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1">
-        <v>950</v>
+        <v>900</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="0"/>
-        <v>-6.9333333333333336</v>
+        <v>-7.3</v>
       </c>
       <c r="P14">
         <v>0.06</v>
       </c>
       <c r="Q14">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>0.43</v>
+        <v>0.27</v>
       </c>
       <c r="E15" s="1">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="F15" s="1">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I15" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="1">
-        <v>200</v>
+        <v>-70</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1">
-        <v>1200</v>
+        <v>950</v>
       </c>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
-        <v>-7.3833333333333337</v>
+        <v>-6.9333333333333336</v>
       </c>
       <c r="P15">
         <v>0.06</v>
       </c>
       <c r="Q15">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>0.43</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D16" s="1">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="E16" s="1">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="F16" s="1">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1">
@@ -1741,7 +1734,7 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" si="0"/>
-        <v>-7.1833333333333345</v>
+        <v>-6.8833333333333337</v>
       </c>
       <c r="P16">
         <v>0.06</v>
@@ -1749,32 +1742,29 @@
       <c r="Q16">
         <v>16</v>
       </c>
-      <c r="R16">
-        <v>0.01</v>
-      </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="D17" s="1">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="E17" s="1">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="F17" s="1">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1">
@@ -1793,7 +1783,7 @@
       </c>
       <c r="N17" s="1">
         <f t="shared" si="0"/>
-        <v>-7.1833333333333327</v>
+        <v>-6.6833333333333345</v>
       </c>
       <c r="P17">
         <v>0.06</v>
@@ -1802,268 +1792,274 @@
         <v>16</v>
       </c>
       <c r="R17">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="E18" s="1">
+        <v>-4</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-4</v>
+      </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="H18" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>200</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="M18" s="1">
+        <v>1200</v>
+      </c>
       <c r="N18" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-6.6833333333333327</v>
+      </c>
+      <c r="P18">
+        <v>0.06</v>
+      </c>
+      <c r="Q18">
+        <v>16</v>
+      </c>
+      <c r="R18">
+        <v>0.02</v>
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.27</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>100</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
       <c r="N19" s="1">
         <f t="shared" si="0"/>
-        <v>-5.5666666666666673</v>
-      </c>
-      <c r="P19">
-        <v>0.06</v>
-      </c>
-      <c r="Q19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
       <c r="N20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-5.5666666666666673</v>
+      </c>
+      <c r="P20">
+        <v>0.06</v>
+      </c>
+      <c r="Q20">
+        <v>9</v>
       </c>
       <c r="S20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.46</v>
-      </c>
-      <c r="E21" s="1">
-        <v>-12</v>
-      </c>
-      <c r="F21" s="1">
-        <v>-14</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>145</v>
-      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="1">
-        <v>2000</v>
-      </c>
+      <c r="M21" s="1"/>
       <c r="N21" s="1">
         <f t="shared" si="0"/>
-        <v>12.033333333333333</v>
-      </c>
-      <c r="P21">
-        <v>0.08</v>
-      </c>
-      <c r="Q21">
-        <v>16.535399999999999</v>
+        <v>0</v>
       </c>
       <c r="S21">
         <f t="shared" si="1"/>
-        <v>0.46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1">
-        <v>0.37</v>
+        <v>0.46</v>
       </c>
       <c r="E22" s="1">
-        <v>-9</v>
+        <v>-12</v>
       </c>
       <c r="F22" s="1">
-        <v>-8</v>
+        <v>-14</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="I22" s="1">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="J22" s="1">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="0"/>
-        <v>7.6999999999999993</v>
+        <v>12.033333333333333</v>
       </c>
       <c r="P22">
         <v>0.08</v>
       </c>
       <c r="Q22">
-        <v>12.795299999999999</v>
+        <v>16.535399999999999</v>
       </c>
       <c r="S22">
         <f t="shared" si="1"/>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>-9</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-8</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="J23" s="1">
+        <v>105</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1">
+        <v>3000</v>
+      </c>
       <c r="N23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.4499999999999993</v>
+      </c>
+      <c r="P23">
+        <v>0.08</v>
+      </c>
+      <c r="Q23">
+        <v>12.795299999999999</v>
       </c>
       <c r="S23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0.24</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>-25</v>
-      </c>
-      <c r="M24">
-        <v>500</v>
-      </c>
       <c r="N24" s="1">
         <f t="shared" si="0"/>
-        <v>-4.8833333333333329</v>
-      </c>
-      <c r="P24">
-        <v>0.06</v>
-      </c>
-      <c r="Q24">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="S24">
         <f t="shared" si="1"/>
-        <v>0.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C25">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0.24</v>
@@ -2075,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2084,11 +2080,11 @@
         <v>-25</v>
       </c>
       <c r="M25">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="N25" s="1">
         <f t="shared" si="0"/>
-        <v>-6.3833333333333329</v>
+        <v>-4.8833333333333329</v>
       </c>
       <c r="P25">
         <v>0.06</v>
@@ -2103,52 +2099,95 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="D26">
-        <v>0.44</v>
+        <v>0.24</v>
       </c>
       <c r="E26">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="I26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>275</v>
+        <v>-25</v>
       </c>
       <c r="M26">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="N26" s="1">
         <f t="shared" si="0"/>
-        <v>-6.7833333333333341</v>
+        <v>-6.3833333333333329</v>
       </c>
       <c r="P26">
         <v>0.06</v>
       </c>
       <c r="Q26">
-        <v>16.5</v>
+        <v>8</v>
       </c>
       <c r="S26">
         <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27">
+        <v>-4</v>
+      </c>
+      <c r="D27">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N27" s="1"/>
+      <c r="E27">
+        <v>-3</v>
+      </c>
+      <c r="F27">
+        <v>-2</v>
+      </c>
+      <c r="H27">
+        <v>-0.1</v>
+      </c>
+      <c r="I27">
+        <v>0.1</v>
+      </c>
+      <c r="J27">
+        <v>275</v>
+      </c>
+      <c r="M27">
+        <v>1000</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.2833333333333341</v>
+      </c>
+      <c r="P27">
+        <v>0.06</v>
+      </c>
+      <c r="Q27">
+        <v>16.5</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="1"/>
+        <v>0.44</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N28" s="1"/>
@@ -2183,7 +2222,11 @@
     <row r="38" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N38" s="1"/>
     </row>
+    <row r="39" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N39" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix 9mm damage 2
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{522B6BD6-586E-4A96-A297-9299D4D507DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F0EF6B83-FE75-421A-AD01-84E8C1C87596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>new</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Izhmash Saiga-9 345mm 9x19</t>
+  </si>
+  <si>
+    <t>dmg</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1074,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,6 +1139,9 @@
       <c r="R2" t="s">
         <v>15</v>
       </c>
+      <c r="T2" t="s">
+        <v>65</v>
+      </c>
       <c r="U2" t="s">
         <v>16</v>
       </c>
@@ -1185,6 +1191,10 @@
         <f>ROUND(Q3*0.023+P3+R3, 2)</f>
         <v>0.16</v>
       </c>
+      <c r="T3">
+        <f>(Q3-5)*0.09/11</f>
+        <v>-4.187536363636361E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1267,6 +1277,10 @@
         <f t="shared" ref="S5:S31" si="1">ROUND(Q5*0.023+P5+R5, 2)</f>
         <v>0.16</v>
       </c>
+      <c r="T5">
+        <f t="shared" ref="T4:T31" si="2">(Q5-5)*0.09/11</f>
+        <v>-4.0909090909090904E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1313,6 +1327,10 @@
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>8.3750727272727272E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1337,7 +1355,7 @@
         <v>-0.2</v>
       </c>
       <c r="I7">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="J7">
         <v>140</v>
@@ -1347,7 +1365,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>-13.633333333333335</v>
+        <v>-13.783333333333335</v>
       </c>
       <c r="P7">
         <v>0.06</v>
@@ -1358,6 +1376,10 @@
       <c r="S7">
         <f t="shared" si="1"/>
         <v>0.43</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>8.9871152727272724E-2</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1393,7 +1415,7 @@
         <v>0.1</v>
       </c>
       <c r="I9">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="J9">
         <v>47</v>
@@ -1403,7 +1425,7 @@
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>1.8066666666666671</v>
+        <v>1.506666666666667</v>
       </c>
       <c r="P9">
         <v>0.06</v>
@@ -1414,6 +1436,10 @@
       <c r="S9">
         <f t="shared" si="1"/>
         <v>0.26</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>3.1567663636363624E-2</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1461,6 +1487,10 @@
         <f t="shared" si="1"/>
         <v>0.19</v>
       </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>6.1202454545454541E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11">
@@ -1520,6 +1550,10 @@
         <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>-1.6363636363636361E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1566,6 +1600,10 @@
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1590,7 +1628,7 @@
         <v>0.12</v>
       </c>
       <c r="I14">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="J14">
         <v>-90</v>
@@ -1600,7 +1638,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>-6.1000000000000005</v>
+        <v>-6.25</v>
       </c>
       <c r="P14">
         <v>0.06</v>
@@ -1611,6 +1649,10 @@
       <c r="S14">
         <f t="shared" si="1"/>
         <v>0.26</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>2.8636363636363637E-2</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1636,7 +1678,7 @@
         <v>0.1</v>
       </c>
       <c r="I15">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="J15">
         <v>-70</v>
@@ -1646,7 +1688,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="0"/>
-        <v>-6.1833333333333336</v>
+        <v>-6.3333333333333339</v>
       </c>
       <c r="P15">
         <v>0.06</v>
@@ -1657,6 +1699,10 @@
       <c r="S15">
         <f t="shared" si="1"/>
         <v>0.27</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>3.2727272727272723E-2</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -1682,7 +1728,7 @@
         <v>0.05</v>
       </c>
       <c r="I16">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="J16">
         <v>200</v>
@@ -1692,7 +1738,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="0"/>
-        <v>-6.8833333333333337</v>
+        <v>-7.0333333333333341</v>
       </c>
       <c r="P16">
         <v>0.06</v>
@@ -1704,8 +1750,12 @@
         <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1728,7 +1778,7 @@
         <v>0.05</v>
       </c>
       <c r="I17">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="J17">
         <v>200</v>
@@ -1738,7 +1788,7 @@
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>-6.6833333333333345</v>
+        <v>-6.8333333333333348</v>
       </c>
       <c r="P17">
         <v>0.06</v>
@@ -1753,8 +1803,12 @@
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17">
+        <f t="shared" si="2"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1777,7 +1831,7 @@
         <v>0.05</v>
       </c>
       <c r="I18">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="J18">
         <v>200</v>
@@ -1787,7 +1841,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="0"/>
-        <v>-6.6833333333333327</v>
+        <v>-6.833333333333333</v>
       </c>
       <c r="P18">
         <v>0.06</v>
@@ -1802,8 +1856,12 @@
         <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <f t="shared" si="2"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1813,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1836,7 +1894,7 @@
         <v>0.1</v>
       </c>
       <c r="I20">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="J20">
         <v>50</v>
@@ -1846,7 +1904,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="0"/>
-        <v>-5.1833333333333336</v>
+        <v>-5.3333333333333339</v>
       </c>
       <c r="P20">
         <v>0.06</v>
@@ -1858,8 +1916,12 @@
         <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <f t="shared" si="2"/>
+        <v>3.5755199999999994E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -1882,7 +1944,7 @@
         <v>0.05</v>
       </c>
       <c r="I21">
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J21">
         <v>90</v>
@@ -1892,7 +1954,7 @@
       </c>
       <c r="N21">
         <f t="shared" si="0"/>
-        <v>-5.2000000000000011</v>
+        <v>-5.5000000000000009</v>
       </c>
       <c r="P21">
         <v>0.06</v>
@@ -1904,8 +1966,12 @@
         <f t="shared" si="1"/>
         <v>0.37</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <f t="shared" si="2"/>
+        <v>7.0222090909090915E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1915,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1938,7 +2004,7 @@
         <v>0.05</v>
       </c>
       <c r="I23">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="J23">
         <v>145</v>
@@ -1948,7 +2014,7 @@
       </c>
       <c r="N23">
         <f t="shared" si="0"/>
-        <v>13.233333333333333</v>
+        <v>13.383333333333333</v>
       </c>
       <c r="P23">
         <v>0.08</v>
@@ -1960,8 +2026,12 @@
         <f t="shared" si="1"/>
         <v>0.46</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <f t="shared" si="2"/>
+        <v>9.4380545454545439E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1984,7 +2054,7 @@
         <v>0.15</v>
       </c>
       <c r="I24">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="J24">
         <v>105</v>
@@ -1994,7 +2064,7 @@
       </c>
       <c r="N24">
         <f t="shared" si="0"/>
-        <v>8.9499999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="P24">
         <v>0.08</v>
@@ -2006,8 +2076,12 @@
         <f t="shared" si="1"/>
         <v>0.37</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <f t="shared" si="2"/>
+        <v>6.3779727272727266E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N25">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2017,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2040,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -2050,7 +2124,7 @@
       </c>
       <c r="N26">
         <f t="shared" si="0"/>
-        <v>-4.2</v>
+        <v>-4.3499999999999996</v>
       </c>
       <c r="P26">
         <v>0.06</v>
@@ -2062,8 +2136,12 @@
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <f t="shared" si="2"/>
+        <v>2.4545454545454547E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2086,7 +2164,7 @@
         <v>0.1</v>
       </c>
       <c r="I27">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -2096,7 +2174,7 @@
       </c>
       <c r="N27">
         <f t="shared" si="0"/>
-        <v>-5.7</v>
+        <v>-5.85</v>
       </c>
       <c r="P27">
         <v>0.06</v>
@@ -2108,8 +2186,12 @@
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <f t="shared" si="2"/>
+        <v>2.4545454545454547E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2132,7 +2214,7 @@
         <v>-0.1</v>
       </c>
       <c r="I28">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="J28">
         <v>275</v>
@@ -2142,7 +2224,7 @@
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
-        <v>-6.2833333333333341</v>
+        <v>-6.4333333333333345</v>
       </c>
       <c r="P28">
         <v>0.06</v>
@@ -2154,8 +2236,12 @@
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28">
+        <f t="shared" si="2"/>
+        <v>9.4090909090909086E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N29">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2165,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -2213,8 +2299,12 @@
         <f t="shared" si="1"/>
         <v>0.19</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <f t="shared" si="2"/>
+        <v>4.187536363636361E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2237,7 +2327,7 @@
         <v>-0.02</v>
       </c>
       <c r="I31">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="J31">
         <v>2</v>
@@ -2250,7 +2340,7 @@
       </c>
       <c r="N31">
         <f>C31-D31*20-E31*0.8-F31*0.6-H31*5+I31*15+J31/300</f>
-        <v>-3.2433333333333332</v>
+        <v>-3.3933333333333335</v>
       </c>
       <c r="P31">
         <v>0.06</v>
@@ -2261,6 +2351,10 @@
       <c r="S31">
         <f t="shared" si="1"/>
         <v>0.21</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="2"/>
+        <v>1.385108181818182E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make glock/wilson heavier, p320 mag funnel lighter
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB76C9A-1D74-4C92-A675-8D49BF7EC3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{76742998-A373-45EA-AB4A-047201FD2202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>new</t>
   </si>
@@ -255,6 +255,18 @@
   </si>
   <si>
     <t>Sig Sauer P320 Full 5.5" Threaded 9x19 Barrel</t>
+  </si>
+  <si>
+    <t>wilson_combat_edc_x9_102mm_9x19_barrel</t>
+  </si>
+  <si>
+    <t>Wilson Combat EDC X9 102mm 9x19</t>
+  </si>
+  <si>
+    <t>wilson_combat_edc_x9_127mm_threaded_9x19_barrel</t>
+  </si>
+  <si>
+    <t>Wilson Combat EDC X9 127mm Threaded 9x19</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1265,7 @@
         <v>1500</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N36" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*7.5+I4*15+J4/300</f>
+        <f t="shared" ref="N4:N39" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*7.5+I4*15+J4/300</f>
         <v>11.06</v>
       </c>
     </row>
@@ -1299,11 +1311,11 @@
         <v>4.5</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S36" si="1">ROUND(Q5*0.023+P5+R5, 2)</f>
+        <f t="shared" ref="S5:S39" si="1">ROUND(Q5*0.023+P5+R5, 2)</f>
         <v>0.16</v>
       </c>
       <c r="T5">
-        <f t="shared" ref="T5:T36" si="2">(Q5-5)*0.09/11</f>
+        <f t="shared" ref="T5:T39" si="2">(Q5-5)*0.09/11</f>
         <v>-4.0909090909090904E-3</v>
       </c>
     </row>
@@ -2594,6 +2606,120 @@
       <c r="T36">
         <f t="shared" si="2"/>
         <v>4.0909090909090904E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="2"/>
+        <v>-4.0909090909090902E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0.16</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>-78</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>-3.46</v>
+      </c>
+      <c r="P38">
+        <v>0.06</v>
+      </c>
+      <c r="Q38">
+        <v>4.0157499999999997</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="2"/>
+        <v>-8.0529545454545472E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39">
+        <v>-1</v>
+      </c>
+      <c r="D39">
+        <v>0.18</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>0.1</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>-44</v>
+      </c>
+      <c r="M39">
+        <v>750</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>-8.2966666666666651</v>
+      </c>
+      <c r="P39">
+        <v>0.06</v>
+      </c>
+      <c r="Q39">
+        <v>5</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
9mm mag weight changes
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76742998-A373-45EA-AB4A-047201FD2202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A308C5-DBFA-4506-A679-851EEB8A466D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1110,7 +1110,7 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1194,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="E3">
         <v>-9</v>
@@ -1216,17 +1216,17 @@
       </c>
       <c r="N3">
         <f>C3-D3*20-E3*0.8-F3*0.6-H3*7.5+I3*15+J3/300</f>
-        <v>12.996666666666666</v>
+        <v>13.596666666666666</v>
       </c>
       <c r="P3">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="Q3">
         <v>4.4881900000000003</v>
       </c>
       <c r="S3">
         <f>ROUND(Q3*0.023+P3+R3, 2)</f>
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="T3">
         <f>(Q3-5)*0.09/11</f>
@@ -1244,7 +1244,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="E4">
         <v>-10</v>
@@ -1266,7 +1266,10 @@
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N39" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*7.5+I4*15+J4/300</f>
-        <v>11.06</v>
+        <v>11.66</v>
+      </c>
+      <c r="P4">
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -1280,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="E5">
         <v>-7</v>
@@ -1302,17 +1305,17 @@
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>7.835</v>
+        <v>8.4350000000000005</v>
       </c>
       <c r="P5">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="Q5">
         <v>4.5</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5:S39" si="1">ROUND(Q5*0.023+P5+R5, 2)</f>
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="T5">
         <f t="shared" ref="T5:T39" si="2">(Q5-5)*0.09/11</f>
@@ -1330,7 +1333,7 @@
         <v>-1</v>
       </c>
       <c r="D6">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="E6">
         <v>-12</v>
@@ -1352,17 +1355,17 @@
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>14.753333333333334</v>
+        <v>15.353333333333333</v>
       </c>
       <c r="P6">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="Q6">
         <v>6.0236200000000002</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
@@ -1380,7 +1383,7 @@
         <v>-25</v>
       </c>
       <c r="D7">
-        <v>0.43</v>
+        <v>0.4</v>
       </c>
       <c r="E7">
         <v>-10</v>
@@ -1402,17 +1405,17 @@
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>-13.283333333333335</v>
+        <v>-12.683333333333334</v>
       </c>
       <c r="P7">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="Q7">
         <v>15.984252</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>0.43</v>
+        <v>0.4</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
@@ -1421,1191 +1424,1207 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="N8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C8-D8*20-E8*0.8-F8*0.6-H8*7.5+I8*15+J8/300</f>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0.03</v>
       </c>
       <c r="S8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>ROUND(Q8*0.023+P8+R8, 2)</f>
+        <v>0.03</v>
+      </c>
+      <c r="T8">
+        <f>(Q8-5)*0.09/11</f>
+        <v>-4.0909090909090902E-2</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>0.26</v>
+        <v>0.11000000000000001</v>
       </c>
       <c r="E9">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="H9">
         <v>0.1</v>
       </c>
       <c r="I9">
+        <v>-0.03</v>
+      </c>
+      <c r="J9">
+        <v>-80</v>
+      </c>
+      <c r="M9">
+        <v>1000</v>
+      </c>
+      <c r="N9">
+        <f>C9-D9*20-E9*0.8-F9*0.6-H9*7.5+I9*15+J9/300</f>
+        <v>-3.8666666666666671</v>
+      </c>
+      <c r="P9">
         <v>0.03</v>
       </c>
-      <c r="J9">
+      <c r="Q9">
+        <v>3.9</v>
+      </c>
+      <c r="S9">
+        <f>ROUND(Q9*0.023+P9+R9, 2)</f>
+        <v>0.12</v>
+      </c>
+      <c r="T9">
+        <f>(Q9-5)*0.09/11</f>
+        <v>-9.0000000000000011E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.13</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.05</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>-50</v>
+      </c>
+      <c r="M10">
+        <v>3000</v>
+      </c>
+      <c r="N10">
+        <f>C10-D10*20-E10*0.8-F10*0.6-H10*7.5+I10*15+J10/300</f>
+        <v>-3.541666666666667</v>
+      </c>
+      <c r="P10">
+        <v>0.03</v>
+      </c>
+      <c r="Q10">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="S10">
+        <f>ROUND(Q10*0.023+P10+R10, 2)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T10">
+        <f>(Q10-5)*0.09/11</f>
+        <v>-3.2727272727272757E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.01</v>
+      </c>
+      <c r="J11">
+        <v>-45</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f>C11-D11*20-E11*0.8-F11*0.6-H11*7.5+I11*15+J11/300</f>
+        <v>-2.8000000000000003</v>
+      </c>
+      <c r="P11">
+        <v>0.03</v>
+      </c>
+      <c r="Q11">
+        <v>4.7</v>
+      </c>
+      <c r="S11">
+        <f>ROUND(Q11*0.023+P11+R11, 2)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T11">
+        <f>(Q11-5)*0.09/11</f>
+        <v>-2.4545454545454527E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12">
+        <v>-3</v>
+      </c>
+      <c r="D12">
+        <v>0.16</v>
+      </c>
+      <c r="E12">
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="H12">
+        <v>-0.1</v>
+      </c>
+      <c r="I12">
+        <v>0.04</v>
+      </c>
+      <c r="J12">
+        <v>-10</v>
+      </c>
+      <c r="M12">
+        <v>1500</v>
+      </c>
+      <c r="N12">
+        <f>C12-D12*20-E12*0.8-F12*0.6-H12*7.5+I12*15+J12/300</f>
+        <v>-3.4833333333333338</v>
+      </c>
+      <c r="P12">
+        <v>0.03</v>
+      </c>
+      <c r="Q12">
+        <v>5.5</v>
+      </c>
+      <c r="S12">
+        <f>ROUND(Q12*0.023+P12+R12, 2)</f>
+        <v>0.16</v>
+      </c>
+      <c r="T12">
+        <f>(Q12-5)*0.09/11</f>
+        <v>4.0909090909090904E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <f>C13-D13*20-E13*0.8-F13*0.6-H13*7.5+I13*15+J13/300</f>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0.03</v>
+      </c>
+      <c r="S13">
+        <f>ROUND(Q13*0.023+P13+R13, 2)</f>
+        <v>0.03</v>
+      </c>
+      <c r="T13">
+        <f>(Q13-5)*0.09/11</f>
+        <v>-4.0909090909090902E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.13</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>-78</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f>C14-D14*20-E14*0.8-F14*0.6-H14*7.5+I14*15+J14/300</f>
+        <v>-2.8600000000000003</v>
+      </c>
+      <c r="P14">
+        <v>0.03</v>
+      </c>
+      <c r="Q14">
+        <v>4.0157499999999997</v>
+      </c>
+      <c r="S14">
+        <f>ROUND(Q14*0.023+P14+R14, 2)</f>
+        <v>0.12</v>
+      </c>
+      <c r="T14">
+        <f>(Q14-5)*0.09/11</f>
+        <v>-8.0529545454545472E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15">
+        <v>-1</v>
+      </c>
+      <c r="D15">
+        <v>0.15</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>0.1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>-44</v>
+      </c>
+      <c r="M15">
+        <v>750</v>
+      </c>
+      <c r="N15">
+        <f>C15-D15*20-E15*0.8-F15*0.6-H15*7.5+I15*15+J15/300</f>
+        <v>-7.6966666666666663</v>
+      </c>
+      <c r="P15">
+        <v>0.03</v>
+      </c>
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="S15">
+        <f>ROUND(Q15*0.023+P15+R15, 2)</f>
+        <v>0.15</v>
+      </c>
+      <c r="T15">
+        <f>(Q15-5)*0.09/11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.26</v>
+      </c>
+      <c r="E17">
+        <v>-3</v>
+      </c>
+      <c r="F17">
+        <v>-7</v>
+      </c>
+      <c r="H17">
+        <v>0.1</v>
+      </c>
+      <c r="I17">
+        <v>0.03</v>
+      </c>
+      <c r="J17">
         <v>47</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="0"/>
         <v>1.256666666666667</v>
       </c>
-      <c r="P9">
-        <v>0.06</v>
-      </c>
-      <c r="Q9">
+      <c r="P17">
+        <v>0.06</v>
+      </c>
+      <c r="Q17">
         <v>8.8582699999999992</v>
       </c>
-      <c r="S9">
+      <c r="S17">
         <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
-      <c r="T9">
+      <c r="T17">
         <f t="shared" si="2"/>
         <v>3.1567663636363624E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C10">
+      <c r="C18">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="D18">
         <v>0.19</v>
       </c>
-      <c r="E10">
+      <c r="E18">
         <v>-1</v>
       </c>
-      <c r="F10">
+      <c r="F18">
         <v>-4</v>
       </c>
-      <c r="H10">
+      <c r="H18">
         <v>0.15</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>80</v>
       </c>
-      <c r="M10">
+      <c r="M18">
         <v>1000</v>
       </c>
-      <c r="N10">
+      <c r="N18">
         <f t="shared" si="0"/>
         <v>0.54166666666666674</v>
       </c>
-      <c r="P10">
-        <v>0.06</v>
-      </c>
-      <c r="Q10">
+      <c r="P18">
+        <v>0.06</v>
+      </c>
+      <c r="Q18">
         <v>5.74803</v>
       </c>
-      <c r="S10">
+      <c r="S18">
         <f t="shared" si="1"/>
         <v>0.19</v>
       </c>
-      <c r="T10">
+      <c r="T18">
         <f t="shared" si="2"/>
         <v>6.1202454545454541E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="N11">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="N19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S11">
+      <c r="P19">
+        <v>0.06</v>
+      </c>
+      <c r="S19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="C12">
+      <c r="C20">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="D20">
         <v>0.13</v>
       </c>
-      <c r="E12">
+      <c r="E20">
         <v>8</v>
       </c>
-      <c r="F12">
+      <c r="F20">
         <v>8</v>
       </c>
-      <c r="H12">
+      <c r="H20">
         <v>0.3</v>
       </c>
-      <c r="I12">
+      <c r="I20">
         <v>-0.15</v>
       </c>
-      <c r="J12">
+      <c r="J20">
         <v>-300</v>
       </c>
-      <c r="M12">
+      <c r="M20">
         <v>750</v>
       </c>
-      <c r="N12">
+      <c r="N20">
         <f t="shared" si="0"/>
         <v>-10.3</v>
       </c>
-      <c r="P12">
-        <v>0.06</v>
-      </c>
-      <c r="Q12">
+      <c r="P20">
+        <v>0.06</v>
+      </c>
+      <c r="Q20">
         <v>3</v>
       </c>
-      <c r="S12">
+      <c r="S20">
         <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
-      <c r="T12">
+      <c r="T20">
         <f t="shared" si="2"/>
         <v>-1.6363636363636361E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C13">
+      <c r="C21">
         <v>7</v>
       </c>
-      <c r="D13">
+      <c r="D21">
         <v>0.18</v>
       </c>
-      <c r="E13">
+      <c r="E21">
         <v>6</v>
       </c>
-      <c r="F13">
+      <c r="F21">
         <v>6</v>
       </c>
-      <c r="H13">
+      <c r="H21">
         <v>0.25</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
         <v>-225</v>
       </c>
-      <c r="M13">
+      <c r="M21">
         <v>800</v>
       </c>
-      <c r="N13">
+      <c r="N21">
         <f t="shared" si="0"/>
         <v>-7.625</v>
       </c>
-      <c r="P13">
-        <v>0.06</v>
-      </c>
-      <c r="Q13">
+      <c r="P21">
+        <v>0.06</v>
+      </c>
+      <c r="Q21">
         <v>5</v>
       </c>
-      <c r="S13">
+      <c r="S21">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
-      <c r="T13">
+      <c r="T21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="C14">
+      <c r="C22">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D22">
         <v>0.26</v>
       </c>
-      <c r="E14">
+      <c r="E22">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="F22">
         <v>2</v>
       </c>
-      <c r="H14">
+      <c r="H22">
         <v>0.12</v>
       </c>
-      <c r="I14">
+      <c r="I22">
         <v>0.03</v>
       </c>
-      <c r="J14">
+      <c r="J22">
         <v>-90</v>
       </c>
-      <c r="M14">
+      <c r="M22">
         <v>900</v>
       </c>
-      <c r="N14">
+      <c r="N22">
         <f t="shared" si="0"/>
         <v>-6.5500000000000007</v>
       </c>
-      <c r="P14">
-        <v>0.06</v>
-      </c>
-      <c r="Q14">
+      <c r="P22">
+        <v>0.06</v>
+      </c>
+      <c r="Q22">
         <v>8.5</v>
       </c>
-      <c r="S14">
+      <c r="S22">
         <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
-      <c r="T14">
+      <c r="T22">
         <f t="shared" si="2"/>
         <v>2.8636363636363637E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="C15">
+      <c r="C23">
         <v>2</v>
       </c>
-      <c r="D15">
+      <c r="D23">
         <v>0.27</v>
       </c>
-      <c r="E15">
+      <c r="E23">
         <v>2</v>
       </c>
-      <c r="F15">
+      <c r="F23">
         <v>2</v>
       </c>
-      <c r="H15">
+      <c r="H23">
         <v>0.1</v>
       </c>
-      <c r="I15">
+      <c r="I23">
         <v>0.04</v>
       </c>
-      <c r="J15">
+      <c r="J23">
         <v>-70</v>
       </c>
-      <c r="M15">
+      <c r="M23">
         <v>950</v>
       </c>
-      <c r="N15">
+      <c r="N23">
         <f t="shared" si="0"/>
         <v>-6.5833333333333339</v>
       </c>
-      <c r="P15">
-        <v>0.06</v>
-      </c>
-      <c r="Q15">
+      <c r="P23">
+        <v>0.06</v>
+      </c>
+      <c r="Q23">
         <v>9</v>
       </c>
-      <c r="S15">
+      <c r="S23">
         <f t="shared" si="1"/>
         <v>0.27</v>
       </c>
-      <c r="T15">
+      <c r="T23">
         <f t="shared" si="2"/>
         <v>3.2727272727272723E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C16">
+      <c r="C24">
         <v>-3</v>
       </c>
-      <c r="D16">
+      <c r="D24">
         <v>0.43</v>
       </c>
-      <c r="E16">
+      <c r="E24">
         <v>-2</v>
       </c>
-      <c r="F16">
+      <c r="F24">
         <v>-2</v>
       </c>
-      <c r="H16">
+      <c r="H24">
         <v>0.05</v>
       </c>
-      <c r="I16">
+      <c r="I24">
         <v>0.09</v>
       </c>
-      <c r="J16">
+      <c r="J24">
         <v>200</v>
       </c>
-      <c r="M16">
+      <c r="M24">
         <v>1200</v>
       </c>
-      <c r="N16">
+      <c r="N24">
         <f t="shared" si="0"/>
         <v>-7.1583333333333341</v>
       </c>
-      <c r="P16">
-        <v>0.06</v>
-      </c>
-      <c r="Q16">
+      <c r="P24">
+        <v>0.06</v>
+      </c>
+      <c r="Q24">
         <v>16</v>
       </c>
-      <c r="S16">
+      <c r="S24">
         <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
-      <c r="T16">
+      <c r="T24">
         <f t="shared" si="2"/>
         <v>0.09</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C17">
+      <c r="C25">
         <v>-4</v>
       </c>
-      <c r="D17">
+      <c r="D25">
         <v>0.44</v>
       </c>
-      <c r="E17">
+      <c r="E25">
         <v>-3</v>
       </c>
-      <c r="F17">
+      <c r="F25">
         <v>-3</v>
       </c>
-      <c r="H17">
+      <c r="H25">
         <v>0.05</v>
       </c>
-      <c r="I17">
+      <c r="I25">
         <v>0.09</v>
       </c>
-      <c r="J17">
+      <c r="J25">
         <v>200</v>
       </c>
-      <c r="M17">
+      <c r="M25">
         <v>1200</v>
       </c>
-      <c r="N17">
+      <c r="N25">
         <f t="shared" si="0"/>
         <v>-6.9583333333333348</v>
       </c>
-      <c r="P17">
-        <v>0.06</v>
-      </c>
-      <c r="Q17">
+      <c r="P25">
+        <v>0.06</v>
+      </c>
+      <c r="Q25">
         <v>16</v>
       </c>
-      <c r="R17">
+      <c r="R25">
         <v>0.01</v>
       </c>
-      <c r="S17">
+      <c r="S25">
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
-      <c r="T17">
+      <c r="T25">
         <f t="shared" si="2"/>
         <v>0.09</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B26" t="s">
         <v>39</v>
       </c>
-      <c r="C18">
+      <c r="C26">
         <v>-5</v>
       </c>
-      <c r="D18">
+      <c r="D26">
         <v>0.46</v>
       </c>
-      <c r="E18">
+      <c r="E26">
         <v>-4</v>
       </c>
-      <c r="F18">
+      <c r="F26">
         <v>-4</v>
       </c>
-      <c r="H18">
+      <c r="H26">
         <v>0.05</v>
       </c>
-      <c r="I18">
+      <c r="I26">
         <v>0.09</v>
       </c>
-      <c r="J18">
+      <c r="J26">
         <v>200</v>
       </c>
-      <c r="M18">
+      <c r="M26">
         <v>1200</v>
       </c>
-      <c r="N18">
+      <c r="N26">
         <f t="shared" si="0"/>
         <v>-6.958333333333333</v>
       </c>
-      <c r="P18">
-        <v>0.06</v>
-      </c>
-      <c r="Q18">
+      <c r="P26">
+        <v>0.06</v>
+      </c>
+      <c r="Q26">
         <v>16</v>
       </c>
-      <c r="R18">
+      <c r="R26">
         <v>0.02</v>
       </c>
-      <c r="S18">
+      <c r="S26">
         <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
-      <c r="T18">
+      <c r="T26">
         <f t="shared" si="2"/>
         <v>0.09</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N19">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S19">
+      <c r="P27">
+        <v>0.06</v>
+      </c>
+      <c r="S27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>61</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B28" t="s">
         <v>62</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="H20">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="H28">
         <v>0.1</v>
       </c>
-      <c r="I20">
+      <c r="I28">
         <v>0.04</v>
       </c>
-      <c r="J20">
+      <c r="J28">
         <v>50</v>
       </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
         <f t="shared" si="0"/>
         <v>-5.5833333333333339</v>
       </c>
-      <c r="P20">
-        <v>0.06</v>
-      </c>
-      <c r="Q20">
+      <c r="P28">
+        <v>0.06</v>
+      </c>
+      <c r="Q28">
         <v>9.3700799999999997</v>
       </c>
-      <c r="S20">
+      <c r="S28">
         <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="T20">
+      <c r="T28">
         <f t="shared" si="2"/>
         <v>3.5755199999999994E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>63</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B29" t="s">
         <v>64</v>
       </c>
-      <c r="C21">
+      <c r="C29">
         <v>-2</v>
       </c>
-      <c r="D21">
+      <c r="D29">
         <v>0.37</v>
       </c>
-      <c r="E21">
+      <c r="E29">
         <v>-2</v>
       </c>
-      <c r="F21">
+      <c r="F29">
         <v>-2</v>
       </c>
-      <c r="H21">
+      <c r="H29">
         <v>0.05</v>
       </c>
-      <c r="I21">
+      <c r="I29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J21">
+      <c r="J29">
         <v>90</v>
       </c>
-      <c r="M21">
+      <c r="M29">
         <v>500</v>
       </c>
-      <c r="N21">
+      <c r="N29">
         <f t="shared" si="0"/>
         <v>-5.6250000000000009</v>
       </c>
-      <c r="P21">
-        <v>0.06</v>
-      </c>
-      <c r="Q21">
+      <c r="P29">
+        <v>0.06</v>
+      </c>
+      <c r="Q29">
         <v>13.582700000000001</v>
       </c>
-      <c r="S21">
+      <c r="S29">
         <f t="shared" si="1"/>
         <v>0.37</v>
       </c>
-      <c r="T21">
+      <c r="T29">
         <f t="shared" si="2"/>
         <v>7.0222090909090915E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N22">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S22">
+      <c r="P30">
+        <v>0.06</v>
+      </c>
+      <c r="S30">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B31" t="s">
         <v>45</v>
       </c>
-      <c r="C23">
+      <c r="C31">
         <v>3</v>
       </c>
-      <c r="D23">
+      <c r="D31">
         <v>0.46</v>
       </c>
-      <c r="E23">
+      <c r="E31">
         <v>-12</v>
       </c>
-      <c r="F23">
+      <c r="F31">
         <v>-14</v>
       </c>
-      <c r="H23">
+      <c r="H31">
         <v>0.05</v>
       </c>
-      <c r="I23">
+      <c r="I31">
         <v>0.09</v>
       </c>
-      <c r="J23">
+      <c r="J31">
         <v>145</v>
       </c>
-      <c r="M23">
+      <c r="M31">
         <v>2000</v>
       </c>
-      <c r="N23">
+      <c r="N31">
         <f t="shared" si="0"/>
         <v>13.258333333333333</v>
       </c>
-      <c r="P23">
-        <v>0.08</v>
-      </c>
-      <c r="Q23">
+      <c r="P31">
+        <v>0.06</v>
+      </c>
+      <c r="Q31">
         <v>16.535399999999999</v>
       </c>
-      <c r="S23">
+      <c r="S31">
         <f t="shared" si="1"/>
-        <v>0.46</v>
-      </c>
-      <c r="T23">
+        <v>0.44</v>
+      </c>
+      <c r="T31">
         <f t="shared" si="2"/>
         <v>9.4380545454545439E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B32" t="s">
         <v>47</v>
       </c>
-      <c r="C24">
+      <c r="C32">
         <v>4</v>
       </c>
-      <c r="D24">
+      <c r="D32">
         <v>0.37</v>
       </c>
-      <c r="E24">
+      <c r="E32">
         <v>-9</v>
       </c>
-      <c r="F24">
+      <c r="F32">
         <v>-8</v>
       </c>
-      <c r="H24">
+      <c r="H32">
         <v>0.15</v>
       </c>
-      <c r="I24">
-        <v>0.06</v>
-      </c>
-      <c r="J24">
+      <c r="I32">
+        <v>0.06</v>
+      </c>
+      <c r="J32">
         <v>105</v>
       </c>
-      <c r="M24">
+      <c r="M32">
         <v>3000</v>
       </c>
-      <c r="N24">
+      <c r="N32">
         <f t="shared" si="0"/>
         <v>8.7249999999999996</v>
       </c>
-      <c r="P24">
-        <v>0.08</v>
-      </c>
-      <c r="Q24">
+      <c r="P32">
+        <v>0.06</v>
+      </c>
+      <c r="Q32">
         <v>12.795299999999999</v>
       </c>
-      <c r="S24">
+      <c r="S32">
         <f t="shared" si="1"/>
-        <v>0.37</v>
-      </c>
-      <c r="T24">
+        <v>0.35</v>
+      </c>
+      <c r="T32">
         <f t="shared" si="2"/>
         <v>6.3779727272727266E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S25">
+      <c r="P33">
+        <v>0.06</v>
+      </c>
+      <c r="S33">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B34" t="s">
         <v>49</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
         <v>0.24</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
         <v>0.03</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="M26">
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="M34">
         <v>500</v>
       </c>
-      <c r="N26">
+      <c r="N34">
         <f t="shared" si="0"/>
         <v>-4.3499999999999996</v>
       </c>
-      <c r="P26">
-        <v>0.06</v>
-      </c>
-      <c r="Q26">
+      <c r="P34">
+        <v>0.06</v>
+      </c>
+      <c r="Q34">
         <v>8</v>
       </c>
-      <c r="S26">
+      <c r="S34">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="T26">
+      <c r="T34">
         <f t="shared" si="2"/>
         <v>2.4545454545454547E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B35" t="s">
         <v>51</v>
       </c>
-      <c r="C27">
+      <c r="C35">
         <v>-1</v>
       </c>
-      <c r="D27">
+      <c r="D35">
         <v>0.24</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="H27">
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <v>0.1</v>
       </c>
-      <c r="I27">
+      <c r="I35">
         <v>0.03</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="M27">
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="M35">
         <v>600</v>
       </c>
-      <c r="N27">
+      <c r="N35">
         <f t="shared" si="0"/>
         <v>-6.1</v>
       </c>
-      <c r="P27">
-        <v>0.06</v>
-      </c>
-      <c r="Q27">
+      <c r="P35">
+        <v>0.06</v>
+      </c>
+      <c r="Q35">
         <v>8</v>
       </c>
-      <c r="S27">
+      <c r="S35">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="T27">
+      <c r="T35">
         <f t="shared" si="2"/>
         <v>2.4545454545454547E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B36" t="s">
         <v>53</v>
       </c>
-      <c r="C28">
+      <c r="C36">
         <v>-4</v>
       </c>
-      <c r="D28">
+      <c r="D36">
         <v>0.44</v>
       </c>
-      <c r="E28">
+      <c r="E36">
         <v>-3</v>
       </c>
-      <c r="F28">
+      <c r="F36">
         <v>-2</v>
       </c>
-      <c r="H28">
+      <c r="H36">
         <v>-0.1</v>
       </c>
-      <c r="I28">
+      <c r="I36">
         <v>0.09</v>
       </c>
-      <c r="J28">
+      <c r="J36">
         <v>275</v>
       </c>
-      <c r="M28">
+      <c r="M36">
         <v>1000</v>
       </c>
-      <c r="N28">
+      <c r="N36">
         <f t="shared" si="0"/>
         <v>-6.1833333333333345</v>
       </c>
-      <c r="P28">
-        <v>0.06</v>
-      </c>
-      <c r="Q28">
+      <c r="P36">
+        <v>0.06</v>
+      </c>
+      <c r="Q36">
         <v>16.5</v>
       </c>
-      <c r="S28">
+      <c r="S36">
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
-      <c r="T28">
+      <c r="T36">
         <f t="shared" si="2"/>
         <v>9.4090909090909086E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0.19</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>-28</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>800</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="0"/>
-        <v>-3.8933333333333331</v>
-      </c>
-      <c r="P30">
-        <v>0.06</v>
-      </c>
-      <c r="Q30">
-        <v>5.5118099999999997</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="1"/>
-        <v>0.19</v>
-      </c>
-      <c r="T30">
-        <f t="shared" si="2"/>
-        <v>4.187536363636361E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31">
-        <v>-1</v>
-      </c>
-      <c r="D31">
-        <v>0.21</v>
-      </c>
-      <c r="E31">
-        <v>-1</v>
-      </c>
-      <c r="F31">
-        <v>-1</v>
-      </c>
-      <c r="H31">
-        <v>-0.02</v>
-      </c>
-      <c r="I31">
-        <v>0.02</v>
-      </c>
-      <c r="J31">
-        <v>2</v>
-      </c>
-      <c r="K31">
-        <v>-0.1</v>
-      </c>
-      <c r="M31">
-        <v>750</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="0"/>
-        <v>-3.3433333333333337</v>
-      </c>
-      <c r="P31">
-        <v>0.06</v>
-      </c>
-      <c r="Q31">
-        <v>6.6929100000000004</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="1"/>
-        <v>0.21</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="2"/>
-        <v>1.385108181818182E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T32">
-        <f t="shared" si="2"/>
-        <v>-4.0909090909090902E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
-      </c>
-      <c r="F33">
-        <v>3</v>
-      </c>
-      <c r="H33">
-        <v>0.1</v>
-      </c>
-      <c r="I33">
-        <v>-0.03</v>
-      </c>
-      <c r="J33">
-        <v>-80</v>
-      </c>
-      <c r="M33">
-        <v>1000</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="0"/>
-        <v>-4.4666666666666668</v>
-      </c>
-      <c r="P33">
-        <v>0.06</v>
-      </c>
-      <c r="Q33">
-        <v>3.9</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="1"/>
-        <v>0.15</v>
-      </c>
-      <c r="T33">
-        <f t="shared" si="2"/>
-        <v>-9.0000000000000011E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>0.16</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>0.05</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>-50</v>
-      </c>
-      <c r="M34">
-        <v>3000</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="0"/>
-        <v>-4.1416666666666666</v>
-      </c>
-      <c r="P34">
-        <v>0.06</v>
-      </c>
-      <c r="Q34">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="S34">
-        <f t="shared" si="1"/>
-        <v>0.17</v>
-      </c>
-      <c r="T34">
-        <f t="shared" si="2"/>
-        <v>-3.2727272727272757E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0.17</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0.01</v>
-      </c>
-      <c r="J35">
-        <v>-45</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="0"/>
-        <v>-3.4000000000000004</v>
-      </c>
-      <c r="P35">
-        <v>0.06</v>
-      </c>
-      <c r="Q35">
-        <v>4.7</v>
-      </c>
-      <c r="S35">
-        <f t="shared" si="1"/>
-        <v>0.17</v>
-      </c>
-      <c r="T35">
-        <f t="shared" si="2"/>
-        <v>-2.4545454545454527E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36">
-        <v>-3</v>
-      </c>
-      <c r="D36">
-        <v>0.19</v>
-      </c>
-      <c r="E36">
-        <v>-1</v>
-      </c>
-      <c r="F36">
-        <v>-1</v>
-      </c>
-      <c r="H36">
-        <v>-0.1</v>
-      </c>
-      <c r="I36">
-        <v>0.04</v>
-      </c>
-      <c r="J36">
-        <v>-10</v>
-      </c>
-      <c r="M36">
-        <v>1500</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="0"/>
-        <v>-4.0833333333333339</v>
-      </c>
-      <c r="P36">
-        <v>0.06</v>
-      </c>
-      <c r="Q36">
-        <v>5.5</v>
-      </c>
-      <c r="S36">
-        <f t="shared" si="1"/>
-        <v>0.19</v>
-      </c>
-      <c r="T36">
-        <f t="shared" si="2"/>
-        <v>4.0909090909090904E-3</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -2613,27 +2632,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="P37">
+        <v>0.06</v>
+      </c>
       <c r="S37">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T37">
-        <f t="shared" si="2"/>
-        <v>-4.0909090909090902E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2648,78 +2666,84 @@
         <v>0</v>
       </c>
       <c r="J38">
-        <v>-78</v>
+        <v>-28</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
       </c>
       <c r="M38">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N38">
         <f t="shared" si="0"/>
-        <v>-3.46</v>
+        <v>-3.8933333333333331</v>
       </c>
       <c r="P38">
         <v>0.06</v>
       </c>
       <c r="Q38">
-        <v>4.0157499999999997</v>
+        <v>5.5118099999999997</v>
       </c>
       <c r="S38">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="T38">
         <f t="shared" si="2"/>
-        <v>-8.0529545454545472E-3</v>
+        <v>4.187536363636361E-3</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C39">
         <v>-1</v>
       </c>
       <c r="D39">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="E39">
+        <v>-1</v>
+      </c>
+      <c r="F39">
+        <v>-1</v>
+      </c>
+      <c r="H39">
+        <v>-0.02</v>
+      </c>
+      <c r="I39">
+        <v>0.02</v>
+      </c>
+      <c r="J39">
         <v>2</v>
       </c>
-      <c r="F39">
-        <v>2</v>
-      </c>
-      <c r="H39">
-        <v>0.1</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>-44</v>
+      <c r="K39">
+        <v>-0.1</v>
       </c>
       <c r="M39">
         <v>750</v>
       </c>
       <c r="N39">
         <f t="shared" si="0"/>
-        <v>-8.2966666666666651</v>
+        <v>-3.3433333333333337</v>
       </c>
       <c r="P39">
         <v>0.06</v>
       </c>
       <c r="Q39">
-        <v>5</v>
+        <v>6.6929100000000004</v>
       </c>
       <c r="S39">
         <f t="shared" si="1"/>
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="T39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.385108181818182E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make aug para mags and shit heavier
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A308C5-DBFA-4506-A679-851EEB8A466D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6185C35-9143-4B34-A097-8F8510856C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1110,7 +1110,7 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,8 +1225,8 @@
         <v>4.4881900000000003</v>
       </c>
       <c r="S3">
-        <f>ROUND(Q3*0.023+P3+R3, 2)</f>
-        <v>0.13</v>
+        <f>ROUND(Q3*0.024+P3+R3, 2)</f>
+        <v>0.14000000000000001</v>
       </c>
       <c r="T3">
         <f>(Q3-5)*0.09/11</f>
@@ -1271,6 +1271,10 @@
       <c r="P4">
         <v>0.03</v>
       </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S39" si="1">ROUND(Q4*0.024+P4+R4, 2)</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1314,8 +1318,8 @@
         <v>4.5</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S39" si="1">ROUND(Q5*0.023+P5+R5, 2)</f>
-        <v>0.13</v>
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
       </c>
       <c r="T5">
         <f t="shared" ref="T5:T39" si="2">(Q5-5)*0.09/11</f>
@@ -1415,7 +1419,7 @@
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
@@ -1424,18 +1428,18 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="N8">
-        <f>C8-D8*20-E8*0.8-F8*0.6-H8*7.5+I8*15+J8/300</f>
+        <f t="shared" ref="N8:N15" si="3">C8-D8*20-E8*0.8-F8*0.6-H8*7.5+I8*15+J8/300</f>
         <v>0</v>
       </c>
       <c r="P8">
         <v>0.03</v>
       </c>
       <c r="S8">
-        <f>ROUND(Q8*0.023+P8+R8, 2)</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="T8">
-        <f>(Q8-5)*0.09/11</f>
+        <f t="shared" ref="T8:T15" si="4">(Q8-5)*0.09/11</f>
         <v>-4.0909090909090902E-2</v>
       </c>
     </row>
@@ -1471,7 +1475,7 @@
         <v>1000</v>
       </c>
       <c r="N9">
-        <f>C9-D9*20-E9*0.8-F9*0.6-H9*7.5+I9*15+J9/300</f>
+        <f t="shared" si="3"/>
         <v>-3.8666666666666671</v>
       </c>
       <c r="P9">
@@ -1481,11 +1485,11 @@
         <v>3.9</v>
       </c>
       <c r="S9">
-        <f>ROUND(Q9*0.023+P9+R9, 2)</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="T9">
-        <f>(Q9-5)*0.09/11</f>
+        <f t="shared" si="4"/>
         <v>-9.0000000000000011E-3</v>
       </c>
     </row>
@@ -1521,7 +1525,7 @@
         <v>3000</v>
       </c>
       <c r="N10">
-        <f>C10-D10*20-E10*0.8-F10*0.6-H10*7.5+I10*15+J10/300</f>
+        <f t="shared" si="3"/>
         <v>-3.541666666666667</v>
       </c>
       <c r="P10">
@@ -1531,11 +1535,11 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="S10">
-        <f>ROUND(Q10*0.023+P10+R10, 2)</f>
+        <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="T10">
-        <f>(Q10-5)*0.09/11</f>
+        <f t="shared" si="4"/>
         <v>-3.2727272727272757E-3</v>
       </c>
     </row>
@@ -1571,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <f>C11-D11*20-E11*0.8-F11*0.6-H11*7.5+I11*15+J11/300</f>
+        <f t="shared" si="3"/>
         <v>-2.8000000000000003</v>
       </c>
       <c r="P11">
@@ -1581,11 +1585,11 @@
         <v>4.7</v>
       </c>
       <c r="S11">
-        <f>ROUND(Q11*0.023+P11+R11, 2)</f>
+        <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="T11">
-        <f>(Q11-5)*0.09/11</f>
+        <f t="shared" si="4"/>
         <v>-2.4545454545454527E-3</v>
       </c>
     </row>
@@ -1621,7 +1625,7 @@
         <v>1500</v>
       </c>
       <c r="N12">
-        <f>C12-D12*20-E12*0.8-F12*0.6-H12*7.5+I12*15+J12/300</f>
+        <f t="shared" si="3"/>
         <v>-3.4833333333333338</v>
       </c>
       <c r="P12">
@@ -1631,28 +1635,28 @@
         <v>5.5</v>
       </c>
       <c r="S12">
-        <f>ROUND(Q12*0.023+P12+R12, 2)</f>
+        <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
       <c r="T12">
-        <f>(Q12-5)*0.09/11</f>
+        <f t="shared" si="4"/>
         <v>4.0909090909090904E-3</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="N13">
-        <f>C13-D13*20-E13*0.8-F13*0.6-H13*7.5+I13*15+J13/300</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P13">
         <v>0.03</v>
       </c>
       <c r="S13">
-        <f>ROUND(Q13*0.023+P13+R13, 2)</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="T13">
-        <f>(Q13-5)*0.09/11</f>
+        <f t="shared" si="4"/>
         <v>-4.0909090909090902E-2</v>
       </c>
     </row>
@@ -1688,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <f>C14-D14*20-E14*0.8-F14*0.6-H14*7.5+I14*15+J14/300</f>
+        <f t="shared" si="3"/>
         <v>-2.8600000000000003</v>
       </c>
       <c r="P14">
@@ -1698,11 +1702,11 @@
         <v>4.0157499999999997</v>
       </c>
       <c r="S14">
-        <f>ROUND(Q14*0.023+P14+R14, 2)</f>
-        <v>0.12</v>
+        <f t="shared" si="1"/>
+        <v>0.13</v>
       </c>
       <c r="T14">
-        <f>(Q14-5)*0.09/11</f>
+        <f t="shared" si="4"/>
         <v>-8.0529545454545472E-3</v>
       </c>
     </row>
@@ -1738,7 +1742,7 @@
         <v>750</v>
       </c>
       <c r="N15">
-        <f>C15-D15*20-E15*0.8-F15*0.6-H15*7.5+I15*15+J15/300</f>
+        <f t="shared" si="3"/>
         <v>-7.6966666666666663</v>
       </c>
       <c r="P15">
@@ -1748,11 +1752,11 @@
         <v>5</v>
       </c>
       <c r="S15">
-        <f>ROUND(Q15*0.023+P15+R15, 2)</f>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
       <c r="T15">
-        <f>(Q15-5)*0.09/11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1809,7 +1813,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="T17">
         <f t="shared" si="2"/>
@@ -1859,7 +1863,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="T18">
         <f t="shared" si="2"/>
@@ -2075,7 +2079,7 @@
       </c>
       <c r="S23">
         <f t="shared" si="1"/>
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="T23">
         <f t="shared" si="2"/>
@@ -2125,7 +2129,7 @@
       </c>
       <c r="S24">
         <f t="shared" si="1"/>
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="T24">
         <f t="shared" si="2"/>
@@ -2178,7 +2182,7 @@
       </c>
       <c r="S25">
         <f t="shared" si="1"/>
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="T25">
         <f t="shared" si="2"/>
@@ -2231,7 +2235,7 @@
       </c>
       <c r="S26">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="T26">
         <f t="shared" si="2"/>
@@ -2344,7 +2348,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="1"/>
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="T29">
         <f t="shared" si="2"/>
@@ -2375,7 +2379,7 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
       <c r="E31">
         <v>-12</v>
@@ -2397,7 +2401,7 @@
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
-        <v>13.258333333333333</v>
+        <v>13.058333333333335</v>
       </c>
       <c r="P31">
         <v>0.06</v>
@@ -2407,7 +2411,7 @@
       </c>
       <c r="S31">
         <f t="shared" si="1"/>
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="T31">
         <f t="shared" si="2"/>
@@ -2425,7 +2429,7 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <v>0.37</v>
+        <v>0.38</v>
       </c>
       <c r="E32">
         <v>-9</v>
@@ -2447,7 +2451,7 @@
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
-        <v>8.7249999999999996</v>
+        <v>8.5250000000000004</v>
       </c>
       <c r="P32">
         <v>0.06</v>
@@ -2457,7 +2461,7 @@
       </c>
       <c r="S32">
         <f t="shared" si="1"/>
-        <v>0.35</v>
+        <v>0.37</v>
       </c>
       <c r="T32">
         <f t="shared" si="2"/>
@@ -2520,7 +2524,7 @@
       </c>
       <c r="S34">
         <f t="shared" si="1"/>
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="T34">
         <f t="shared" si="2"/>
@@ -2570,7 +2574,7 @@
       </c>
       <c r="S35">
         <f t="shared" si="1"/>
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="T35">
         <f t="shared" si="2"/>
@@ -2620,7 +2624,7 @@
       </c>
       <c r="S36">
         <f t="shared" si="1"/>
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="T36">
         <f t="shared" si="2"/>
@@ -2739,7 +2743,7 @@
       </c>
       <c r="S39">
         <f t="shared" si="1"/>
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="T39">
         <f t="shared" si="2"/>

</xml_diff>